<commit_message>
Added little more details to flowchart. Started on resolution/execution script.
</commit_message>
<xml_diff>
--- a/BarrelRoll/Assets/Documentation/FlowChart.xlsx
+++ b/BarrelRoll/Assets/Documentation/FlowChart.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GameDevProjects\ProjectBarrelRoll\BarrelRoll_Repo\BarrelRoll\Assets\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C90D4589-E411-4E4C-9E29-474314936F1F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3521F871-FD4A-42C8-81C5-372D05785E44}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18960" windowHeight="8985" xr2:uid="{1A359DE2-5036-4B9F-9F05-28DD652830AD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18960" windowHeight="8985" activeTab="3" xr2:uid="{1A359DE2-5036-4B9F-9F05-28DD652830AD}"/>
   </bookViews>
   <sheets>
     <sheet name="MainGameLoop" sheetId="1" r:id="rId1"/>
     <sheet name="AttackOptions" sheetId="2" r:id="rId2"/>
     <sheet name="EvadeOptions" sheetId="3" r:id="rId3"/>
+    <sheet name="PowerCircle" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -4532,6 +4533,847 @@
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>141994</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>180094</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8426C54E-D4D9-410A-BE87-BC1589EEF3E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4438650" y="1238250"/>
+          <a:ext cx="1227844" cy="1227844"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>65793</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>180093</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2A5CC30-D02D-484A-AA89-A9A25792D1A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6400801" y="65793"/>
+          <a:ext cx="1257300" cy="1257300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>151518</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>56268</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7158FBE6-AFBB-48CD-8A65-466D99865ADB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8401050" y="1066800"/>
+          <a:ext cx="1275468" cy="1275468"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>132469</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>56269</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38F1C7CE-FBB0-4036-9C09-52E355050F08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6410325" y="4323469"/>
+          <a:ext cx="1257300" cy="1257300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>170568</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>122943</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70FC22B6-A5A2-438A-8014-1055814FCB38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4362450" y="3218568"/>
+          <a:ext cx="1285875" cy="1285875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>189619</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>161043</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65688DEE-C84F-4217-877A-A2CB95CB1186}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8420100" y="3248024"/>
+          <a:ext cx="1294519" cy="1294519"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>137672</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>51506</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Connector: Curved 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC0ABF5B-A3AB-4882-A37B-D2119C8CC095}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="1"/>
+          <a:endCxn id="12" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="4362450" y="1852172"/>
+          <a:ext cx="76200" cy="2009334"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 400000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>99572</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>65792</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Connector: Curved 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{685F1F29-3A79-4040-966E-DFCB937528D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="0"/>
+          <a:endCxn id="4" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1" flipV="1">
+          <a:off x="5454783" y="-336419"/>
+          <a:ext cx="1172457" cy="1976879"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -19498"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>52387</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>122943</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>56269</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Connector: Curved 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3911F8E-B01A-4100-9A39-4DE2EA6EDE93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="12" idx="2"/>
+          <a:endCxn id="10" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="5484018" y="4025812"/>
+          <a:ext cx="1076326" cy="2033587"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 121239"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>161043</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>113859</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>56269</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Connector: Curved 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F838743-12DE-4FDC-A2A3-D2007B71A439}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="10" idx="2"/>
+          <a:endCxn id="14" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="7534054" y="4047463"/>
+          <a:ext cx="1038226" cy="2028385"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -22018"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>151518</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>180534</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>189619</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>85284</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Connector: Curved 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A0C695F-B9D1-48D5-8DA5-ACFA169A50C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="14" idx="3"/>
+          <a:endCxn id="8" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9676518" y="1704534"/>
+          <a:ext cx="38101" cy="2190750"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -599984"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>171452</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>65793</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>85285</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Connector: Curved 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E95EAAD4-09EF-4999-BB86-AE539C9B264D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="0"/>
+          <a:endCxn id="6" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="7533615" y="-438370"/>
+          <a:ext cx="1001007" cy="2009333"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 122837"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C773A894-5CC0-4296-96AA-4E974D52C350}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5457825" y="2105025"/>
+          <a:ext cx="3305175" cy="1476375"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="triangle" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>180093</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>132469</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Straight Arrow Connector 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F394A043-D881-4B36-92FF-1A4CB878A57A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="10" idx="0"/>
+          <a:endCxn id="6" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="7029451" y="1323093"/>
+          <a:ext cx="9524" cy="3000376"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Straight Arrow Connector 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFBCEDA0-DFC6-4F94-A6C9-66CC67632973}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5362576" y="2085975"/>
+          <a:ext cx="3400424" cy="1457325"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent4"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -4842,7 +5684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56E1557-6DEA-461B-B66C-4EF35316B7F3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="AY52" sqref="AY52"/>
     </sheetView>
   </sheetViews>
@@ -4875,4 +5717,19 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9D762E-A9E8-46A8-9B2A-E1272DFEF19E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="BE10" sqref="BE10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Can manually trigger barrelRoll, calculates card resolution, swaps the ship models and health UI, and other stuff. Figuring out how I want to add to the deck and whatnot. Thinking of using deck.Add(Resourses.Load("Card_Name") as Card), but I'm not sure if that's the way to go about it.
</commit_message>
<xml_diff>
--- a/BarrelRoll/Assets/Documentation/FlowChart.xlsx
+++ b/BarrelRoll/Assets/Documentation/FlowChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GameDevProjects\ProjectBarrelRoll\BarrelRoll_Repo\BarrelRoll\Assets\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3521F871-FD4A-42C8-81C5-372D05785E44}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940E055A-BAE1-4E62-ABBF-564465BD205A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18960" windowHeight="8985" activeTab="3" xr2:uid="{1A359DE2-5036-4B9F-9F05-28DD652830AD}"/>
   </bookViews>
@@ -4599,15 +4599,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>114301</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>65793</xdr:rowOff>
+      <xdr:colOff>165101</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
-      <xdr:colOff>38101</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>180093</xdr:rowOff>
+      <xdr:colOff>88901</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4636,7 +4636,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6400801" y="65793"/>
+          <a:off x="6451601" y="482600"/>
           <a:ext cx="1257300" cy="1257300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4699,15 +4699,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>132469</xdr:rowOff>
+      <xdr:colOff>111125</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>5469</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>56269</xdr:rowOff>
+      <xdr:colOff>34925</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>119769</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4736,7 +4736,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6410325" y="4323469"/>
+          <a:off x="6397625" y="4005969"/>
           <a:ext cx="1257300" cy="1257300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4911,14 +4911,14 @@
     <xdr:from>
       <xdr:col>26</xdr:col>
       <xdr:colOff>99572</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>65792</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>31751</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4936,12 +4936,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1" flipV="1">
-          <a:off x="5454783" y="-336419"/>
-          <a:ext cx="1172457" cy="1976879"/>
+          <a:off x="5688587" y="-153415"/>
+          <a:ext cx="755650" cy="2027679"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -19498"/>
+            <a:gd name="adj1" fmla="val -30252"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -4977,9 +4977,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>56269</xdr:rowOff>
+      <xdr:colOff>168274</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>119769</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4997,12 +4997,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="5484018" y="4025812"/>
-          <a:ext cx="1076326" cy="2033587"/>
+          <a:off x="5636418" y="3873412"/>
+          <a:ext cx="758826" cy="2020887"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 121239"/>
+            <a:gd name="adj1" fmla="val 130125"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -5032,15 +5032,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>180974</xdr:colOff>
+      <xdr:colOff>168274</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>161043</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>47</xdr:col>
       <xdr:colOff>113859</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>56269</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>119769</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5058,12 +5058,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="7534054" y="4047463"/>
-          <a:ext cx="1038226" cy="2028385"/>
+          <a:off x="7686454" y="3882363"/>
+          <a:ext cx="720726" cy="2041085"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -22018"/>
+            <a:gd name="adj1" fmla="val -31718"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -5153,14 +5153,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>171452</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>65793</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>31751</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>47</xdr:col>
-      <xdr:colOff>85285</xdr:colOff>
+      <xdr:colOff>85284</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -5180,12 +5180,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="7533615" y="-438370"/>
-          <a:ext cx="1001007" cy="2009333"/>
+          <a:off x="7767418" y="-204567"/>
+          <a:ext cx="584200" cy="1958533"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 122837"/>
+            <a:gd name="adj1" fmla="val 139130"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -5274,15 +5274,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>171451</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>180093</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>132469</xdr:rowOff>
+      <xdr:colOff>168275</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>31751</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>5469</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5299,9 +5299,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="7029451" y="1323093"/>
-          <a:ext cx="9524" cy="3000376"/>
+        <a:xfrm flipV="1">
+          <a:off x="7026275" y="1739900"/>
+          <a:ext cx="53976" cy="2266069"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5723,8 +5723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9D762E-A9E8-46A8-9B2A-E1272DFEF19E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BE10" sqref="BE10"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="BH16" sqref="BH16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>